<commit_message>
improve generate raw score
</commit_message>
<xml_diff>
--- a/web/App_Data/template/laporan-sesi-ujian.xlsx
+++ b/web/App_Data/template/laporan-sesi-ujian.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Nama</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Q25</t>
+  </si>
+  <si>
+    <t>Nama Program</t>
   </si>
 </sst>
 </file>
@@ -562,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Z6" sqref="Z6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,7 +607,9 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
template excel raw score
</commit_message>
<xml_diff>
--- a/web/App_Data/template/laporan-sesi-ujian.xlsx
+++ b/web/App_Data/template/laporan-sesi-ujian.xlsx
@@ -223,7 +223,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -243,15 +243,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -563,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,34 +575,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
     </row>
-    <row r="2" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,85 +740,59 @@
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
     </row>
-    <row r="5" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
+    <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
     </row>
-    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
+    <row r="6" spans="1:28" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:28" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-    </row>
-    <row r="8" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:X1"/>

</xml_diff>

<commit_message>
#193 Tukar nama Worksheet mengikut nama ujian, tukar nama column Nama Program > Kod Program dan tukar title Excelsheet kepada format yang disarankan dalam form "Laporan Raw Score Excel".
</commit_message>
<xml_diff>
--- a/web/App_Data/template/laporan-sesi-ujian.xlsx
+++ b/web/App_Data/template/laporan-sesi-ujian.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24684" windowHeight="11208"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="11205"/>
   </bookViews>
   <sheets>
     <sheet name="IPU" sheetId="1" r:id="rId1"/>
@@ -110,7 +110,7 @@
     <t>Q25</t>
   </si>
   <si>
-    <t>Nama Program</t>
+    <t>Kod Program</t>
   </si>
 </sst>
 </file>
@@ -246,11 +246,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -565,44 +565,44 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="1" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
     </row>
-    <row r="2" spans="1:28" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +688,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -714,7 +714,7 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -740,7 +740,7 @@
       <c r="W4" s="7"/>
       <c r="X4" s="7"/>
     </row>
-    <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -766,7 +766,7 @@
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
     </row>
-    <row r="6" spans="1:28" s="10" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -792,7 +792,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:X1"/>

</xml_diff>

<commit_message>
#193 tambah tab untuk setiap ujian
</commit_message>
<xml_diff>
--- a/web/App_Data/template/laporan-sesi-ujian.xlsx
+++ b/web/App_Data/template/laporan-sesi-ujian.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\rep.generic.psikometrik\web\App_Data\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nazrul\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="11205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="11205" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="IPU" sheetId="1" r:id="rId1"/>
+    <sheet name="IPU" sheetId="2" r:id="rId1"/>
+    <sheet name="IBK" sheetId="1" r:id="rId2"/>
+    <sheet name="IP" sheetId="3" r:id="rId3"/>
+    <sheet name="PPKP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
   <si>
     <t>Nama</t>
   </si>
@@ -564,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
@@ -800,4 +803,730 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:X1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+    </row>
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+    </row>
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+    </row>
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#193 Tukar format excel dan tukar format nombor soalan supaya papar nombor seksyen
</commit_message>
<xml_diff>
--- a/web/App_Data/template/laporan-sesi-ujian.xlsx
+++ b/web/App_Data/template/laporan-sesi-ujian.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nazrul\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\rep.generic.psikometrik\web\App_Data\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="11205" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24690" windowHeight="11205"/>
   </bookViews>
   <sheets>
-    <sheet name="IPU" sheetId="2" r:id="rId1"/>
-    <sheet name="IBK" sheetId="1" r:id="rId2"/>
-    <sheet name="IP" sheetId="3" r:id="rId3"/>
-    <sheet name="PPKP" sheetId="4" r:id="rId4"/>
+    <sheet name="Home" sheetId="5" r:id="rId1"/>
+    <sheet name="IPU" sheetId="2" r:id="rId2"/>
+    <sheet name="IBK" sheetId="1" r:id="rId3"/>
+    <sheet name="IP" sheetId="3" r:id="rId4"/>
+    <sheet name="PPKP" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="30">
   <si>
     <t>Nama</t>
   </si>
@@ -113,14 +114,17 @@
     <t>Q25</t>
   </si>
   <si>
-    <t>Kod Program</t>
+    <t>Sila pilih ujian berkenanaan</t>
+  </si>
+  <si>
+    <t>Nama Ujian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +161,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -226,7 +238,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -251,6 +263,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -565,6 +578,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -578,39 +610,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -805,11 +837,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
@@ -820,39 +852,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -1047,7 +1079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
@@ -1062,39 +1094,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -1289,7 +1321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
@@ -1304,39 +1336,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
     </row>
     <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Tambah tab ujian dan betulkan arahan pad tab HOME. Pastikan save pada tab HOME.
</commit_message>
<xml_diff>
--- a/web/App_Data/template/laporan-sesi-ujian.xlsx
+++ b/web/App_Data/template/laporan-sesi-ujian.xlsx
@@ -17,6 +17,9 @@
     <sheet name="IBK" sheetId="1" r:id="rId3"/>
     <sheet name="IP" sheetId="3" r:id="rId4"/>
     <sheet name="PPKP" sheetId="4" r:id="rId5"/>
+    <sheet name="ISO" sheetId="7" r:id="rId6"/>
+    <sheet name="UKHLP" sheetId="10" r:id="rId7"/>
+    <sheet name="UKBP" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="30">
   <si>
     <t>Nama</t>
   </si>
@@ -114,10 +117,10 @@
     <t>Q25</t>
   </si>
   <si>
-    <t>Sila pilih ujian berkenanaan</t>
-  </si>
-  <si>
     <t>Nama Ujian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sila Pilih Tab Ujian </t>
   </si>
 </sst>
 </file>
@@ -580,13 +583,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -642,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -884,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -1126,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -1368,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -1561,4 +1566,730 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+    </row>
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:X1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+    </row>
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+    </row>
+    <row r="2" spans="1:28" s="8" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+    </row>
+    <row r="4" spans="1:28" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+    </row>
+    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+    </row>
+    <row r="6" spans="1:28" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>